<commit_message>
Final Logistic Regression Model trained
</commit_message>
<xml_diff>
--- a/Data/Consolidated Expense Tagging.xlsx
+++ b/Data/Consolidated Expense Tagging.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9236" uniqueCount="3721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8984" uniqueCount="3604">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -10832,357 +10832,6 @@
   </si>
   <si>
     <t xml:space="preserve">Sundari Saree Private Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vision Express </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vijay Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optical Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spectacle Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Popular Optical Stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A. Tanna &amp; Sons opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dev Optics </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kulkarni Brothers Opticians And Contact Lens Clinic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optical Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eyemax Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lenskart.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">President Insight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fantasy Optics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eye Contact Optician</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titan Eyeplus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marol Eye Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shah Optical Gallery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DGT Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerard Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gala Optics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHHEDA OPTICAL MART</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITAN EYEWEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pretty Vision optical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GKB Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTIC ZONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alankar Optical Centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mark Optical </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alankar Eye Care</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lawrence and Mayo Opticians,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chashma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vision Express India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eye Max Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ashoka Optical Centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dayal Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Optical Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rama Vision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruby &amp; Ruby Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vikram Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optical Plaza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kuwar Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I Care Opticals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Siddharth Vision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chopra Optical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Om Opticians</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mochi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khadim's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lakhani Shoe Centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sen Fo &amp; Company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titas Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calcutta Shoe Co</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metro Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D° SHEEN &amp; CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shaby footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandal Shop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sreeleathers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boot Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elite Shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woodland </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hamlyn Grande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hush Puppies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kowloon Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Exclusive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khadim's Showroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Henry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shoes Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Woodland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamal &amp; Kamal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jenn Kee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajanta Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kalindi shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radu Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOOTSEE PLUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krishna Shoe Stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bata Shoe Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Footsee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kamala Shoe House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Merlin Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Babu Shoe Stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIKE4.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jolly Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skechers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bansdroni Bata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classic Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reliance Footprint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZOHRA FOOTWEAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K. M. Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.D.Shoe House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First Step Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milan Shoe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sahara Shoe Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fancy Shoe Stores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khadim's - Lake Town</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elite Shoe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trendz Footware</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ad Maestro Shoe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Skechers </t>
-  </si>
-  <si>
-    <t xml:space="preserve">India Shoe House</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Heels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feet Candy Shoe Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shoe Market</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoes store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branded Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delco Shoes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taj Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHOE FACTORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FANCY SHOE EMPORIUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Subhash Footwear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Shoe Market</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dada Shoe Store</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sreeleathers Showroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balujas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guru kirpa custom Shop</t>
   </si>
 </sst>
 </file>
@@ -11302,11 +10951,11 @@
   </sheetPr>
   <dimension ref="A1:B4618"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4579" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4541" activeCellId="0" sqref="B4541:B4618"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4470" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4488" activeCellId="0" sqref="C4488"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.91"/>
@@ -47248,1013 +46897,383 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="4493" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4493" s="2" t="s">
-        <v>3604</v>
-      </c>
-      <c r="B4493" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4494" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4494" s="2" t="s">
-        <v>3606</v>
-      </c>
-      <c r="B4494" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4495" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4495" s="2" t="s">
-        <v>3607</v>
-      </c>
-      <c r="B4495" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4496" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4496" s="2" t="s">
-        <v>3608</v>
-      </c>
-      <c r="B4496" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4497" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4497" s="2" t="s">
-        <v>3609</v>
-      </c>
-      <c r="B4497" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4498" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4498" s="2" t="s">
-        <v>3610</v>
-      </c>
-      <c r="B4498" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4499" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4499" s="2" t="s">
-        <v>3611</v>
-      </c>
-      <c r="B4499" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4500" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4500" s="2" t="s">
-        <v>3612</v>
-      </c>
-      <c r="B4500" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4501" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4501" s="2" t="s">
-        <v>3613</v>
-      </c>
-      <c r="B4501" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4502" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4502" s="2" t="s">
-        <v>3614</v>
-      </c>
-      <c r="B4502" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4503" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4503" s="2" t="s">
-        <v>3615</v>
-      </c>
-      <c r="B4503" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4504" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4504" s="2" t="s">
-        <v>3616</v>
-      </c>
-      <c r="B4504" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4505" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4505" s="2" t="s">
-        <v>3617</v>
-      </c>
-      <c r="B4505" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4506" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4506" s="2" t="s">
-        <v>3618</v>
-      </c>
-      <c r="B4506" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4507" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4507" s="2" t="s">
-        <v>3619</v>
-      </c>
-      <c r="B4507" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4508" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4508" s="2" t="s">
-        <v>3620</v>
-      </c>
-      <c r="B4508" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4509" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4509" s="2" t="s">
-        <v>3621</v>
-      </c>
-      <c r="B4509" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4510" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4510" s="2" t="s">
-        <v>3622</v>
-      </c>
-      <c r="B4510" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4511" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4511" s="2" t="s">
-        <v>3623</v>
-      </c>
-      <c r="B4511" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4512" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4512" s="2" t="s">
-        <v>3624</v>
-      </c>
-      <c r="B4512" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4513" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4513" s="2" t="s">
-        <v>3625</v>
-      </c>
-      <c r="B4513" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4514" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4514" s="2" t="s">
-        <v>3626</v>
-      </c>
-      <c r="B4514" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4515" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4515" s="2" t="s">
-        <v>3627</v>
-      </c>
-      <c r="B4515" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4516" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4516" s="2" t="s">
-        <v>3628</v>
-      </c>
-      <c r="B4516" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4517" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4517" s="2" t="s">
-        <v>3629</v>
-      </c>
-      <c r="B4517" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4518" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4518" s="2" t="s">
-        <v>3606</v>
-      </c>
-      <c r="B4518" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4519" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4519" s="2" t="s">
-        <v>3630</v>
-      </c>
-      <c r="B4519" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4520" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4520" s="2" t="s">
-        <v>3631</v>
-      </c>
-      <c r="B4520" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4521" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4521" s="2" t="s">
-        <v>3632</v>
-      </c>
-      <c r="B4521" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4522" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4522" s="2" t="s">
-        <v>3633</v>
-      </c>
-      <c r="B4522" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4523" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4523" s="2" t="s">
-        <v>3634</v>
-      </c>
-      <c r="B4523" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4524" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4524" s="2" t="s">
-        <v>3635</v>
-      </c>
-      <c r="B4524" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4525" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4525" s="2" t="s">
-        <v>3636</v>
-      </c>
-      <c r="B4525" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4526" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4526" s="2" t="s">
-        <v>3637</v>
-      </c>
-      <c r="B4526" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4527" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4527" s="2" t="s">
-        <v>3638</v>
-      </c>
-      <c r="B4527" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4528" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4528" s="2" t="s">
-        <v>3639</v>
-      </c>
-      <c r="B4528" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4529" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4529" s="2" t="s">
-        <v>3640</v>
-      </c>
-      <c r="B4529" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4530" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4530" s="2" t="s">
-        <v>3638</v>
-      </c>
-      <c r="B4530" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4531" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4531" s="2" t="s">
-        <v>3641</v>
-      </c>
-      <c r="B4531" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4532" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4532" s="2" t="s">
-        <v>3642</v>
-      </c>
-      <c r="B4532" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4533" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4533" s="2" t="s">
-        <v>3643</v>
-      </c>
-      <c r="B4533" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4534" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4534" s="2" t="s">
-        <v>3613</v>
-      </c>
-      <c r="B4534" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4535" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4535" s="2" t="s">
-        <v>3644</v>
-      </c>
-      <c r="B4535" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4536" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4536" s="2" t="s">
-        <v>3645</v>
-      </c>
-      <c r="B4536" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4537" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4537" s="2" t="s">
-        <v>3646</v>
-      </c>
-      <c r="B4537" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4538" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4538" s="2" t="s">
-        <v>3647</v>
-      </c>
-      <c r="B4538" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4539" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4539" s="2" t="s">
-        <v>3648</v>
-      </c>
-      <c r="B4539" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4540" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4540" s="2" t="s">
-        <v>3649</v>
-      </c>
-      <c r="B4540" s="0" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="4541" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4541" s="2" t="s">
-        <v>3650</v>
-      </c>
-      <c r="B4541" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4542" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4542" s="2" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B4542" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4543" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4543" s="2" t="s">
-        <v>3653</v>
-      </c>
-      <c r="B4543" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4544" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4544" s="2" t="s">
-        <v>3654</v>
-      </c>
-      <c r="B4544" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4545" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4545" s="2" t="s">
-        <v>3655</v>
-      </c>
-      <c r="B4545" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4546" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4546" s="2" t="s">
-        <v>3656</v>
-      </c>
-      <c r="B4546" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4547" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4547" s="2" t="s">
-        <v>3657</v>
-      </c>
-      <c r="B4547" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4548" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4548" s="2" t="s">
-        <v>3658</v>
-      </c>
-      <c r="B4548" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4549" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4549" s="2" t="s">
-        <v>3659</v>
-      </c>
-      <c r="B4549" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4550" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4550" s="2" t="s">
-        <v>3660</v>
-      </c>
-      <c r="B4550" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4551" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4551" s="2" t="s">
-        <v>3661</v>
-      </c>
-      <c r="B4551" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4552" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4552" s="2" t="s">
-        <v>3662</v>
-      </c>
-      <c r="B4552" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4553" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4553" s="2" t="s">
-        <v>3663</v>
-      </c>
-      <c r="B4553" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4554" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4554" s="2" t="s">
-        <v>3664</v>
-      </c>
-      <c r="B4554" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4555" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4555" s="2" t="s">
-        <v>3654</v>
-      </c>
-      <c r="B4555" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4556" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4556" s="2" t="s">
-        <v>3658</v>
-      </c>
-      <c r="B4556" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4557" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4557" s="2" t="s">
-        <v>3665</v>
-      </c>
-      <c r="B4557" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4558" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4558" s="2" t="s">
-        <v>3666</v>
-      </c>
-      <c r="B4558" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4559" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4559" s="2" t="s">
-        <v>3667</v>
-      </c>
-      <c r="B4559" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4560" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4560" s="2" t="s">
-        <v>3668</v>
-      </c>
-      <c r="B4560" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4561" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4561" s="2" t="s">
-        <v>3669</v>
-      </c>
-      <c r="B4561" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4562" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4562" s="2" t="s">
-        <v>3670</v>
-      </c>
-      <c r="B4562" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4563" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4563" s="2" t="s">
-        <v>3671</v>
-      </c>
-      <c r="B4563" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4564" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4564" s="2" t="s">
-        <v>3672</v>
-      </c>
-      <c r="B4564" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4565" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4565" s="2" t="s">
-        <v>3664</v>
-      </c>
-      <c r="B4565" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4566" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4566" s="2" t="s">
-        <v>3673</v>
-      </c>
-      <c r="B4566" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4567" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4567" s="2" t="s">
-        <v>3665</v>
-      </c>
-      <c r="B4567" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4568" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4568" s="2" t="s">
-        <v>3674</v>
-      </c>
-      <c r="B4568" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4569" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4569" s="2" t="s">
-        <v>3675</v>
-      </c>
-      <c r="B4569" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4570" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4570" s="2" t="s">
-        <v>3676</v>
-      </c>
-      <c r="B4570" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4571" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4571" s="2" t="s">
-        <v>3677</v>
-      </c>
-      <c r="B4571" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4572" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4572" s="2" t="s">
-        <v>3678</v>
-      </c>
-      <c r="B4572" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4573" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4573" s="2" t="s">
-        <v>3679</v>
-      </c>
-      <c r="B4573" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4574" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4574" s="2" t="s">
-        <v>3680</v>
-      </c>
-      <c r="B4574" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4575" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4575" s="2" t="s">
-        <v>3681</v>
-      </c>
-      <c r="B4575" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4576" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4576" s="2" t="s">
-        <v>3682</v>
-      </c>
-      <c r="B4576" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4577" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4577" s="2" t="s">
-        <v>3683</v>
-      </c>
-      <c r="B4577" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4578" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4578" s="2" t="s">
-        <v>3684</v>
-      </c>
-      <c r="B4578" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4579" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4579" s="2" t="s">
-        <v>3685</v>
-      </c>
-      <c r="B4579" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4580" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4580" s="2" t="s">
-        <v>3686</v>
-      </c>
-      <c r="B4580" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4581" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4581" s="2" t="s">
-        <v>3687</v>
-      </c>
-      <c r="B4581" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4582" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4582" s="2" t="s">
-        <v>3688</v>
-      </c>
-      <c r="B4582" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4583" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4583" s="2" t="s">
-        <v>3689</v>
-      </c>
-      <c r="B4583" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4584" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4584" s="2" t="s">
-        <v>3690</v>
-      </c>
-      <c r="B4584" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4585" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4585" s="2" t="s">
-        <v>3691</v>
-      </c>
-      <c r="B4585" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4586" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4586" s="2" t="s">
-        <v>3692</v>
-      </c>
-      <c r="B4586" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4587" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4587" s="2" t="s">
-        <v>3693</v>
-      </c>
-      <c r="B4587" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4588" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4588" s="2" t="s">
-        <v>3694</v>
-      </c>
-      <c r="B4588" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4589" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4589" s="2" t="s">
-        <v>3695</v>
-      </c>
-      <c r="B4589" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4590" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4590" s="2" t="s">
-        <v>3696</v>
-      </c>
-      <c r="B4590" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4591" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4591" s="2" t="s">
-        <v>3697</v>
-      </c>
-      <c r="B4591" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4592" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4592" s="2" t="s">
-        <v>3674</v>
-      </c>
-      <c r="B4592" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4593" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4593" s="2" t="s">
-        <v>3682</v>
-      </c>
-      <c r="B4593" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4594" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4594" s="2" t="s">
-        <v>3698</v>
-      </c>
-      <c r="B4594" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4595" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4595" s="2" t="s">
-        <v>3699</v>
-      </c>
-      <c r="B4595" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4596" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4596" s="2" t="s">
-        <v>3700</v>
-      </c>
-      <c r="B4596" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4597" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4597" s="2" t="s">
-        <v>3663</v>
-      </c>
-      <c r="B4597" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4598" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4598" s="2" t="s">
-        <v>3701</v>
-      </c>
-      <c r="B4598" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4599" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4599" s="2" t="s">
-        <v>3702</v>
-      </c>
-      <c r="B4599" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4600" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4600" s="2" t="s">
-        <v>3703</v>
-      </c>
-      <c r="B4600" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4601" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4601" s="2" t="s">
-        <v>3704</v>
-      </c>
-      <c r="B4601" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4602" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4602" s="2" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B4602" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4603" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4603" s="2" t="s">
-        <v>3705</v>
-      </c>
-      <c r="B4603" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4604" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4604" s="2" t="s">
-        <v>3706</v>
-      </c>
-      <c r="B4604" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4605" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4605" s="2" t="s">
-        <v>3707</v>
-      </c>
-      <c r="B4605" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4606" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4606" s="2" t="s">
-        <v>3708</v>
-      </c>
-      <c r="B4606" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4607" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4607" s="2" t="s">
-        <v>3709</v>
-      </c>
-      <c r="B4607" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4608" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4608" s="2" t="s">
-        <v>3710</v>
-      </c>
-      <c r="B4608" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4609" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4609" s="2" t="s">
-        <v>3711</v>
-      </c>
-      <c r="B4609" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4610" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4610" s="2" t="s">
-        <v>3712</v>
-      </c>
-      <c r="B4610" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4611" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4611" s="2" t="s">
-        <v>3713</v>
-      </c>
-      <c r="B4611" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4612" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4612" s="2" t="s">
-        <v>3714</v>
-      </c>
-      <c r="B4612" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4613" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4613" s="2" t="s">
-        <v>3715</v>
-      </c>
-      <c r="B4613" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4614" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4614" s="2" t="s">
-        <v>3716</v>
-      </c>
-      <c r="B4614" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4615" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4615" s="2" t="s">
-        <v>3717</v>
-      </c>
-      <c r="B4615" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4616" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4616" s="2" t="s">
-        <v>3718</v>
-      </c>
-      <c r="B4616" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4617" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4617" s="2" t="s">
-        <v>3719</v>
-      </c>
-      <c r="B4617" s="0" t="s">
-        <v>3651</v>
-      </c>
-    </row>
-    <row r="4618" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4618" s="2" t="s">
-        <v>3720</v>
-      </c>
-      <c r="B4618" s="0" t="s">
-        <v>3651</v>
-      </c>
+    <row r="4493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4493" s="2"/>
+    </row>
+    <row r="4494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4494" s="2"/>
+    </row>
+    <row r="4495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4495" s="2"/>
+    </row>
+    <row r="4496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4496" s="2"/>
+    </row>
+    <row r="4497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4497" s="2"/>
+    </row>
+    <row r="4498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4498" s="2"/>
+    </row>
+    <row r="4499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4499" s="2"/>
+    </row>
+    <row r="4500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4500" s="2"/>
+    </row>
+    <row r="4501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4501" s="2"/>
+    </row>
+    <row r="4502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4502" s="2"/>
+    </row>
+    <row r="4503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4503" s="2"/>
+    </row>
+    <row r="4504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4504" s="2"/>
+    </row>
+    <row r="4505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4505" s="2"/>
+    </row>
+    <row r="4506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4506" s="2"/>
+    </row>
+    <row r="4507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4507" s="2"/>
+    </row>
+    <row r="4508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4508" s="2"/>
+    </row>
+    <row r="4509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4509" s="2"/>
+    </row>
+    <row r="4510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4510" s="2"/>
+    </row>
+    <row r="4511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4511" s="2"/>
+    </row>
+    <row r="4512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4512" s="2"/>
+    </row>
+    <row r="4513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4513" s="2"/>
+    </row>
+    <row r="4514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4514" s="2"/>
+    </row>
+    <row r="4515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4515" s="2"/>
+    </row>
+    <row r="4516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4516" s="2"/>
+    </row>
+    <row r="4517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4517" s="2"/>
+    </row>
+    <row r="4518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4518" s="2"/>
+    </row>
+    <row r="4519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4519" s="2"/>
+    </row>
+    <row r="4520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4520" s="2"/>
+    </row>
+    <row r="4521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4521" s="2"/>
+    </row>
+    <row r="4522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4522" s="2"/>
+    </row>
+    <row r="4523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4523" s="2"/>
+    </row>
+    <row r="4524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4524" s="2"/>
+    </row>
+    <row r="4525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4525" s="2"/>
+    </row>
+    <row r="4526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4526" s="2"/>
+    </row>
+    <row r="4527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4527" s="2"/>
+    </row>
+    <row r="4528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4528" s="2"/>
+    </row>
+    <row r="4529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4529" s="2"/>
+    </row>
+    <row r="4530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4530" s="2"/>
+    </row>
+    <row r="4531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4531" s="2"/>
+    </row>
+    <row r="4532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4532" s="2"/>
+    </row>
+    <row r="4533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4533" s="2"/>
+    </row>
+    <row r="4534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4534" s="2"/>
+    </row>
+    <row r="4535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4535" s="2"/>
+    </row>
+    <row r="4536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4536" s="2"/>
+    </row>
+    <row r="4537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4537" s="2"/>
+    </row>
+    <row r="4538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4538" s="2"/>
+    </row>
+    <row r="4539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4539" s="2"/>
+    </row>
+    <row r="4540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4540" s="2"/>
+    </row>
+    <row r="4541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4541" s="2"/>
+    </row>
+    <row r="4542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4542" s="2"/>
+    </row>
+    <row r="4543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4543" s="2"/>
+    </row>
+    <row r="4544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4544" s="2"/>
+    </row>
+    <row r="4545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4545" s="2"/>
+    </row>
+    <row r="4546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4546" s="2"/>
+    </row>
+    <row r="4547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4547" s="2"/>
+    </row>
+    <row r="4548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4548" s="2"/>
+    </row>
+    <row r="4549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4549" s="2"/>
+    </row>
+    <row r="4550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4550" s="2"/>
+    </row>
+    <row r="4551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4551" s="2"/>
+    </row>
+    <row r="4552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4552" s="2"/>
+    </row>
+    <row r="4553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4553" s="2"/>
+    </row>
+    <row r="4554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4554" s="2"/>
+    </row>
+    <row r="4555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4555" s="2"/>
+    </row>
+    <row r="4556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4556" s="2"/>
+    </row>
+    <row r="4557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4557" s="2"/>
+    </row>
+    <row r="4558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4558" s="2"/>
+    </row>
+    <row r="4559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4559" s="2"/>
+    </row>
+    <row r="4560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4560" s="2"/>
+    </row>
+    <row r="4561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4561" s="2"/>
+    </row>
+    <row r="4562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4562" s="2"/>
+    </row>
+    <row r="4563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4563" s="2"/>
+    </row>
+    <row r="4564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4564" s="2"/>
+    </row>
+    <row r="4565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4565" s="2"/>
+    </row>
+    <row r="4566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4566" s="2"/>
+    </row>
+    <row r="4567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4567" s="2"/>
+    </row>
+    <row r="4568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4568" s="2"/>
+    </row>
+    <row r="4569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4569" s="2"/>
+    </row>
+    <row r="4570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4570" s="2"/>
+    </row>
+    <row r="4571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4571" s="2"/>
+    </row>
+    <row r="4572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4572" s="2"/>
+    </row>
+    <row r="4573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4573" s="2"/>
+    </row>
+    <row r="4574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4574" s="2"/>
+    </row>
+    <row r="4575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4575" s="2"/>
+    </row>
+    <row r="4576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4576" s="2"/>
+    </row>
+    <row r="4577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4577" s="2"/>
+    </row>
+    <row r="4578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4578" s="2"/>
+    </row>
+    <row r="4579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4579" s="2"/>
+    </row>
+    <row r="4580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4580" s="2"/>
+    </row>
+    <row r="4581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4581" s="2"/>
+    </row>
+    <row r="4582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4582" s="2"/>
+    </row>
+    <row r="4583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4583" s="2"/>
+    </row>
+    <row r="4584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4584" s="2"/>
+    </row>
+    <row r="4585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4585" s="2"/>
+    </row>
+    <row r="4586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4586" s="2"/>
+    </row>
+    <row r="4587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4587" s="2"/>
+    </row>
+    <row r="4588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4588" s="2"/>
+    </row>
+    <row r="4589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4589" s="2"/>
+    </row>
+    <row r="4590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4590" s="2"/>
+    </row>
+    <row r="4591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4591" s="2"/>
+    </row>
+    <row r="4592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4592" s="2"/>
+    </row>
+    <row r="4593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4593" s="2"/>
+    </row>
+    <row r="4594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4594" s="2"/>
+    </row>
+    <row r="4595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4595" s="2"/>
+    </row>
+    <row r="4596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4596" s="2"/>
+    </row>
+    <row r="4597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4597" s="2"/>
+    </row>
+    <row r="4598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4598" s="2"/>
+    </row>
+    <row r="4599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4599" s="2"/>
+    </row>
+    <row r="4600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4600" s="2"/>
+    </row>
+    <row r="4601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4601" s="2"/>
+    </row>
+    <row r="4602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4602" s="2"/>
+    </row>
+    <row r="4603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4603" s="2"/>
+    </row>
+    <row r="4604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4604" s="2"/>
+    </row>
+    <row r="4605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4605" s="2"/>
+    </row>
+    <row r="4606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4606" s="2"/>
+    </row>
+    <row r="4607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4607" s="2"/>
+    </row>
+    <row r="4608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4608" s="2"/>
+    </row>
+    <row r="4609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4609" s="2"/>
+    </row>
+    <row r="4610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4610" s="2"/>
+    </row>
+    <row r="4611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4611" s="2"/>
+    </row>
+    <row r="4612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4612" s="2"/>
+    </row>
+    <row r="4613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4613" s="2"/>
+    </row>
+    <row r="4614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4614" s="2"/>
+    </row>
+    <row r="4615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4615" s="2"/>
+    </row>
+    <row r="4616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4616" s="2"/>
+    </row>
+    <row r="4617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4617" s="2"/>
+    </row>
+    <row r="4618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4618" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>